<commit_message>
put nonsense email addresses in sample subscriptions file
</commit_message>
<xml_diff>
--- a/files/subscriptions_example.xlsx
+++ b/files/subscriptions_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b064b1ad65f4371e/Training/PyProjects/EmailNewsFeed/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{779A076F-F1A2-43DE-9E8C-3D1A8146F634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D97EC3E8-9C86-45BE-B60C-67725A08F469}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{779A076F-F1A2-43DE-9E8C-3D1A8146F634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CD24794-5D45-4274-9F17-E5B337D6EF34}"/>
   <bookViews>
     <workbookView xWindow="4785" yWindow="1170" windowWidth="20685" windowHeight="14355" xr2:uid="{29F88AFA-134A-4825-963A-01402C9FA212}"/>
   </bookViews>
@@ -36,20 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Steven</t>
   </si>
   <si>
-    <t>Elkind</t>
-  </si>
-  <si>
-    <t>saelkind@gmail.com</t>
-  </si>
-  <si>
-    <t>selkind@aol.com</t>
-  </si>
-  <si>
     <t>Linsday Stirling, James Taylor, Star Trek</t>
   </si>
   <si>
@@ -74,10 +65,22 @@
     <t>Lucas</t>
   </si>
   <si>
-    <t>s_elkind@yahoo.com</t>
-  </si>
-  <si>
-    <t>Ukraine, Micropython, Tesla, Subaru, Lindsey Stirling</t>
+    <t>Gribnich</t>
+  </si>
+  <si>
+    <t>sgribnich345@gmail.com</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>ssmitty_do_not_use.@aol.com</t>
+  </si>
+  <si>
+    <t>Ukraine, Micropython, Tesla, Subaru, Lindsey Stirling, Raspberry Pi</t>
+  </si>
+  <si>
+    <t>jlucas.foobar@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -458,29 +461,29 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="51.140625" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" customWidth="1"/>
+    <col min="4" max="4" width="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -488,13 +491,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -502,24 +505,24 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
         <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>

</xml_diff>